<commit_message>
[ISP-2] Esportazione serie soriche per Punti di prelievo
</commit_message>
<xml_diff>
--- a/forcaster-ATM/forcaster-ATM-app/src/baf-configuration/25_Workflow.xlsx
+++ b/forcaster-ATM/forcaster-ATM-app/src/baf-configuration/25_Workflow.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Workflow" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Parameters!$A$1:$E$36</definedName>
   </definedNames>
-  <calcPr calcId="0" refMode="R1C1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -221,7 +221,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="85">
   <si>
     <t>Action</t>
   </si>
@@ -337,9 +337,6 @@
     <t>weightMainAttribute</t>
   </si>
   <si>
-    <t>ALL</t>
-  </si>
-  <si>
     <t>A_PuntoDiPrelievo</t>
   </si>
   <si>
@@ -401,6 +398,85 @@
   </si>
   <si>
     <t>IMP_TOT_PRELEVATO_Mix</t>
+  </si>
+  <si>
+    <t>QuantiliPrelevato</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>writeQuantileSeriesToTimeseriesAttribute (ForecasterLibrary)</t>
+  </si>
+  <si>
+    <t>Param1</t>
+  </si>
+  <si>
+    <t>PUNTI DI PRELIEVO</t>
+  </si>
+  <si>
+    <t>Param2</t>
+  </si>
+  <si>
+    <t>Param3</t>
+  </si>
+  <si>
+    <t>Param4</t>
+  </si>
+  <si>
+    <t>1;2;5;95;98;99</t>
+  </si>
+  <si>
+    <t>Param5</t>
+  </si>
+  <si>
+    <t>QuantilePrelevato1;QuantilePrelevato2;QuantilePrelevato3;QuantilePrelevato95;QuantilePrelevato98;QuantilePrelevato99</t>
+  </si>
+  <si>
+    <t>Param6</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>QuantiliPrelevatoAggr</t>
+  </si>
+  <si>
+    <t>PrelevatoAggr</t>
+  </si>
+  <si>
+    <t>QuantiliVersamento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QuantileVersamento1;QuantileVersamento2;QuantileVersamento5;QuantileVersamento95;QuantileVersamento98;QuantileVersamento99
+</t>
+  </si>
+  <si>
+    <t>QuantilePrelevato1;QuantilePrelevato2;QuantilePrelevato5;QuantilePrelevato95;QuantilePrelevato98;QuantilePrelevato99</t>
+  </si>
+  <si>
+    <t>Step 9</t>
+  </si>
+  <si>
+    <t>Step 10</t>
+  </si>
+  <si>
+    <t>Step 11</t>
+  </si>
+  <si>
+    <t>Step 12</t>
+  </si>
+  <si>
+    <t>Export PuntidiPrelievo TS</t>
+  </si>
+  <si>
+    <t>Aggregate ID</t>
+  </si>
+  <si>
+    <t>startDate</t>
+  </si>
+  <si>
+    <t>endDate</t>
   </si>
 </sst>
 </file>
@@ -598,7 +674,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -663,6 +739,9 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -917,6 +996,102 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9563100"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9534525"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -932,7 +1107,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1524000</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -975,7 +1150,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1524000</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1023,7 +1198,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1524000</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1071,7 +1246,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1524000</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1119,7 +1294,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1524000</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1133,6 +1308,102 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="10372725" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 7"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10372725" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="AutoShape 7"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10372725" cy="9496425"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1397,6 +1668,102 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 3"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="AutoShape 3"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9467850"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1605,6 +1972,102 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="5" name="AutoShape 3"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 3"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="AutoShape 3"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1903,10 +2366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1930,6 +2393,30 @@
         <v>14</v>
       </c>
     </row>
+    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1939,10 +2426,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1978,22 +2465,22 @@
         <v>8</v>
       </c>
       <c r="I1" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="21" t="s">
-        <v>42</v>
-      </c>
       <c r="K1" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="21" t="s">
-        <v>42</v>
-      </c>
       <c r="M1" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="N1" s="21" t="s">
         <v>41</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -2035,7 +2522,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -2085,13 +2572,13 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -2099,14 +2586,142 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>50</v>
-      </c>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="25"/>
+    </row>
+    <row r="15" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="26"/>
+    </row>
+    <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2117,10 +2732,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -2167,7 +2782,7 @@
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
         <v>27</v>
@@ -2181,10 +2796,10 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -2198,7 +2813,7 @@
         <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -2212,7 +2827,7 @@
         <v>29</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -2226,7 +2841,7 @@
         <v>30</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -2290,7 +2905,7 @@
         <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -2304,7 +2919,7 @@
         <v>29</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -2318,7 +2933,7 @@
         <v>30</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -2382,7 +2997,7 @@
         <v>28</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -2396,7 +3011,7 @@
         <v>29</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -2410,7 +3025,7 @@
         <v>30</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -2488,7 +3103,7 @@
         <v>37</v>
       </c>
       <c r="D27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -2496,10 +3111,10 @@
         <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D28" t="s">
         <v>27</v>
@@ -2510,13 +3125,13 @@
         <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -2524,13 +3139,13 @@
         <v>14</v>
       </c>
       <c r="B30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" t="s">
         <v>51</v>
       </c>
-      <c r="C30" t="s">
-        <v>52</v>
-      </c>
       <c r="D30" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -2538,13 +3153,13 @@
         <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -2552,49 +3167,49 @@
         <v>14</v>
       </c>
       <c r="B32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C32" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" t="s">
         <v>54</v>
       </c>
-      <c r="D32" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" t="s">
-        <v>51</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="D33" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" t="s">
         <v>55</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B34" t="s">
-        <v>51</v>
-      </c>
-      <c r="C34" t="s">
-        <v>56</v>
-      </c>
       <c r="D34" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>14</v>
       </c>
       <c r="B35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C35" t="s">
         <v>33</v>
@@ -2603,18 +3218,570 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>14</v>
       </c>
       <c r="B36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D36" s="1">
         <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D37" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="E37" s="26"/>
+    </row>
+    <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D38" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" s="26"/>
+    </row>
+    <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="E39" s="26"/>
+    </row>
+    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="D40" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="E40" s="26"/>
+    </row>
+    <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="E41" s="26"/>
+    </row>
+    <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E42" s="26"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D43" s="26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D44" s="26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="D45" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B46" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="D46" s="26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C47" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D47" s="26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B48" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="D48" s="26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B49" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D49" s="26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B50" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D50" s="26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B51" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C51" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="D51" s="26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B52" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="D52" s="26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B53" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D53" s="26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B54" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C54" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="D54" s="26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C55" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D55" s="26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B56" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C56" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D56" s="26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B57" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C57" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="D57" s="26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B58" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C58" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="D58" s="26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B59" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C59" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D59" s="26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B60" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C60" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="D60" s="26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B61" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C61" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D61" s="26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B62" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C62" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D62" s="26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B63" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C63" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="D63" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B64" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C64" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="D64" s="26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B65" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C65" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D65" s="26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B66" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C66" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="D66" s="26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B67" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C67" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D67" s="26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B68" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C68" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D68" s="26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B69" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C69" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="D69" s="26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B70" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C70" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="D70" s="26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B71" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C71" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D71" s="26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B72" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C72" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="D72" s="26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B73" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C73" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B74" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C74" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="D74" s="1">
+        <v>-365</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B75" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C75" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D75" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>